<commit_message>
changes to TestNG file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DsAlgo_TestData.xlsx
+++ b/src/test/resources/TestData/DsAlgo_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7763D7E3-2CC4-491A-8D3D-F17BC935B1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{324A1C77-84B9-4B64-A6FD-42E34FBDF429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valid_Login" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Array" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E18"/>
+  <oleSize ref="A1:J11"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataChecksum="2RqX7NmqtzoDWSFeiwngA9pRnP1hB2Vhhj4HR5Y8uCc="/>
@@ -1896,7 +1896,7 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -7490,7 +7490,7 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
incorporated review comments in framework
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DsAlgo_TestData.xlsx
+++ b/src/test/resources/TestData/DsAlgo_TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{324A1C77-84B9-4B64-A6FD-42E34FBDF429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8E85B12F-9E0C-4953-9584-5EBEC4BB57F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valid_Login" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Array" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J11"/>
+  <oleSize ref="A1:E18"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataChecksum="2RqX7NmqtzoDWSFeiwngA9pRnP1hB2Vhhj4HR5Y8uCc="/>
@@ -1896,7 +1896,7 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -7490,7 +7490,9 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
initial commit - 1
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DsAlgo_TestData.xlsx
+++ b/src/test/resources/TestData/DsAlgo_TestData.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8E85B12F-9E0C-4953-9584-5EBEC4BB57F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\DsAlgoTestNG\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82199B0D-B4EE-4126-B499-992CD479F6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valid_Login" sheetId="1" r:id="rId1"/>
@@ -18,7 +23,6 @@
     <sheet name="Array" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E18"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataChecksum="2RqX7NmqtzoDWSFeiwngA9pRnP1hB2Vhhj4HR5Y8uCc="/>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="97">
   <si>
     <t>username</t>
   </si>
@@ -261,9 +265,6 @@
 print(my_list</t>
   </si>
   <si>
-    <t>SyntaxError: EOF in multi-line statement on line 4</t>
-  </si>
-  <si>
     <t>fruits = ["apple", "banana", "cherry", "date"]
 fruits.remove("banana")
 print(fruits)</t>
@@ -313,28 +314,6 @@
   </si>
   <si>
     <t>Some Tests failed. Please review code</t>
-  </si>
-  <si>
-    <t>def search(input_list, num): 
-if(num in input_list):
-print("Element Found")
-\b
-\b
-else:
-print("Not Found")
-\b
-\b
-\b
-\b
-search([12, 23, 45, 67, 6, 90] , 25)</t>
-  </si>
-  <si>
-    <t>Not Found</t>
-  </si>
-  <si>
-    <t>def search(lst, value):
-  return value in lst
- print(search([12, 23, 45, 67, 6, 90], 12)) #</t>
   </si>
   <si>
     <t>def search(input_list, num): 
@@ -428,17 +407,6 @@
     <t>SyntaxError: bad input on line 3</t>
   </si>
   <si>
-    <t xml:space="preserve">def sortedSquares(nums):
-\b
-\b
-\b
-\b
-return sorted(x**2 for x in nums)
-nums = [-4, -1, 0, 3, 10]
-result = sortedSquares(nums)
-print(result) </t>
-  </si>
-  <si>
     <t>[0, 1, 9, 16, 100]</t>
   </si>
   <si>
@@ -466,12 +434,29 @@
 result = sortedSquares(nums)
 print(result) # Output: [0, 1, 9, 16, 100]</t>
   </si>
+  <si>
+    <t>SyntaxError: EOF in multi-line statement on line 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def sortedSquares(nums):
+return sorted(x**2 for x in nums)
+nums = [-4, -1, 0, 3, 10]
+result = sortedSquares(nums)
+print(result) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">def sortedSquares(nums):
+  return sorted(x**2 for x in nums)
+nums = [-4, -1, 0, 3, 10]
+result = sortedSquares(nums)
+print(result) </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -559,6 +544,18 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -595,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -640,6 +637,12 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7490,7 +7493,7 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -8569,9 +8572,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C1000"/>
+  <dimension ref="A1:C998"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -8622,176 +8627,158 @@
         <v>69</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="C5" s="22"/>
     </row>
     <row r="6" spans="1:3" ht="46.5" customHeight="1">
       <c r="A6" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>71</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>72</v>
       </c>
       <c r="C6" s="22"/>
     </row>
     <row r="7" spans="1:3" ht="58.5" customHeight="1">
       <c r="A7" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="C7" s="22"/>
     </row>
     <row r="8" spans="1:3" ht="71.25" customHeight="1">
       <c r="A8" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>74</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>75</v>
       </c>
       <c r="C8" s="22"/>
     </row>
     <row r="9" spans="1:3" ht="63" customHeight="1">
       <c r="A9" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="19" t="s">
         <v>76</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>77</v>
       </c>
       <c r="C9" s="22"/>
     </row>
     <row r="10" spans="1:3" ht="156.75" customHeight="1">
       <c r="A10" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>78</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>79</v>
       </c>
       <c r="C10" s="22"/>
     </row>
     <row r="11" spans="1:3" ht="156.75" customHeight="1">
       <c r="A11" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="22"/>
     </row>
     <row r="12" spans="1:3" ht="162" customHeight="1">
       <c r="A12" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="C12" s="22"/>
+    </row>
+    <row r="13" spans="1:3" ht="259.5" customHeight="1">
+      <c r="A13" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="B13" s="23" t="s">
         <v>83</v>
       </c>
+      <c r="C13" s="22"/>
     </row>
-    <row r="13" spans="1:3" ht="162" customHeight="1">
-      <c r="A13" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="162" customHeight="1">
+    <row r="14" spans="1:3" ht="259.5" customHeight="1">
       <c r="A14" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C14" s="22"/>
     </row>
-    <row r="15" spans="1:3" ht="259.5" customHeight="1">
+    <row r="15" spans="1:3" ht="256.5" customHeight="1">
       <c r="A15" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>85</v>
       </c>
       <c r="C15" s="22"/>
     </row>
-    <row r="16" spans="1:3" ht="259.5" customHeight="1">
+    <row r="16" spans="1:3" ht="112.5" customHeight="1">
       <c r="A16" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>80</v>
+      <c r="B16" s="25" t="s">
+        <v>83</v>
       </c>
       <c r="C16" s="22"/>
     </row>
-    <row r="17" spans="1:3" ht="256.5" customHeight="1">
+    <row r="17" spans="1:3" ht="112.5" customHeight="1">
       <c r="A17" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C17" s="22"/>
     </row>
-    <row r="18" spans="1:3" ht="112.5" customHeight="1">
+    <row r="18" spans="1:3" ht="103.5" customHeight="1">
       <c r="A18" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" s="23">
-        <v>2</v>
+        <v>88</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>89</v>
       </c>
       <c r="C18" s="22"/>
     </row>
-    <row r="19" spans="1:3" ht="112.5" customHeight="1">
-      <c r="A19" s="21" t="s">
+    <row r="19" spans="1:3" ht="138" customHeight="1">
+      <c r="A19" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="C19" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="118.5" customHeight="1">
+      <c r="A20" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="22"/>
-    </row>
-    <row r="20" spans="1:3" ht="103.5" customHeight="1">
-      <c r="A20" s="21" t="s">
+      <c r="B20" s="19" t="s">
         <v>92</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>93</v>
       </c>
       <c r="C20" s="22"/>
     </row>
-    <row r="21" spans="1:3" ht="138" customHeight="1">
+    <row r="21" spans="1:3" ht="127.5" customHeight="1">
       <c r="A21" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="C21" s="22"/>
     </row>
-    <row r="22" spans="1:3" ht="118.5" customHeight="1">
-      <c r="A22" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="22"/>
-    </row>
-    <row r="23" spans="1:3" ht="127.5" customHeight="1">
-      <c r="A23" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="22"/>
-    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="24" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="25" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="26" spans="1:3" ht="15.75" customHeight="1"/>
@@ -9767,10 +9754,8 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding home, login and DS
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DsAlgo_TestData.xlsx
+++ b/src/test/resources/TestData/DsAlgo_TestData.xlsx
@@ -1,24 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8E85B12F-9E0C-4953-9584-5EBEC4BB57F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Valid_Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Login" sheetId="2" r:id="rId2"/>
-    <sheet name="Register" sheetId="3" r:id="rId3"/>
-    <sheet name="Linked_List" sheetId="4" r:id="rId4"/>
-    <sheet name="Graph" sheetId="5" r:id="rId5"/>
-    <sheet name="Tree" sheetId="6" r:id="rId6"/>
-    <sheet name="TryEditor" sheetId="7" r:id="rId7"/>
-    <sheet name="Array" sheetId="8" r:id="rId8"/>
+    <sheet state="visible" name="Valid_Login" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Login" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Register" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Linked_List" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Graph" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Tree" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="TryEditor" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="Array" sheetId="8" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:E18"/>
+  <definedNames/>
+  <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataChecksum="2RqX7NmqtzoDWSFeiwngA9pRnP1hB2Vhhj4HR5Y8uCc="/>
@@ -141,18 +136,18 @@
   <si>
     <r>
       <rPr>
-        <sz val="10"/>
+        <rFont val="Arial"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <sz val="10.0"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Arial"/>
         <b/>
-        <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <sz val="12.0"/>
       </rPr>
       <t>OutPut Result</t>
     </r>
@@ -470,93 +465,82 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="14">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF467886"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF467886"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="13.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="13.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="&quot;Aptos Narrow&quot;"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -565,17 +549,11 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -589,78 +567,101 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+  <cellXfs count="23">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -850,26 +851,21 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="6" width="12.6328125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -877,7 +873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -885,20 +881,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="3" ht="15.75" customHeight="1"/>
+    <row r="4" ht="15.75" customHeight="1"/>
+    <row r="5" ht="15.75" customHeight="1"/>
+    <row r="6" ht="15.75" customHeight="1"/>
+    <row r="7" ht="15.75" customHeight="1"/>
+    <row r="8" ht="15.75" customHeight="1"/>
+    <row r="9" ht="15.75" customHeight="1"/>
+    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1"/>
+    <row r="12" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -1884,26 +1880,25 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="6" width="12.6328125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1911,17 +1906,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1929,7 +1924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1937,17 +1932,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="6" ht="15.75" customHeight="1"/>
+    <row r="7" ht="15.75" customHeight="1"/>
+    <row r="8" ht="15.75" customHeight="1"/>
+    <row r="9" ht="15.75" customHeight="1"/>
+    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1"/>
+    <row r="12" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -2933,31 +2928,31 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" customWidth="1"/>
-    <col min="3" max="3" width="19.08984375" customWidth="1"/>
-    <col min="4" max="4" width="34.90625" customWidth="1"/>
-    <col min="5" max="5" width="50.26953125" customWidth="1"/>
-    <col min="6" max="6" width="12.6328125" customWidth="1"/>
+    <col customWidth="1" min="2" max="2" width="18.5"/>
+    <col customWidth="1" min="3" max="3" width="19.13"/>
+    <col customWidth="1" min="4" max="4" width="34.88"/>
+    <col customWidth="1" min="5" max="5" width="50.25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2974,7 +2969,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2985,9 +2980,9 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2">
-        <v>8767686667</v>
+        <v>8.767686667E9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -2996,7 +2991,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3009,7 +3004,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -3021,7 +3016,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -3041,7 +3036,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -3061,7 +3056,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1">
+    <row r="8" ht="15.75" customHeight="1">
       <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
@@ -3078,7 +3073,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1">
+    <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>21</v>
@@ -3096,7 +3091,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1">
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -3115,15 +3110,15 @@
       <c r="F10" s="6"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1">
+    <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="8">
-        <v>987654321</v>
+        <v>9.87654321E8</v>
       </c>
       <c r="C11" s="8">
-        <v>987654321</v>
+        <v>9.87654321E8</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>26</v>
@@ -3135,7 +3130,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1">
+    <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -3155,7 +3150,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1">
+    <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -3172,7 +3167,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1">
+    <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -3190,7 +3185,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1">
+    <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -3207,47 +3202,47 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1">
+    <row r="16" ht="15.75" customHeight="1">
       <c r="F16" s="4"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="6:8" ht="15.75" customHeight="1">
+    <row r="17" ht="15.75" customHeight="1">
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="6:8" ht="15.75" customHeight="1">
+    <row r="18" ht="15.75" customHeight="1">
       <c r="F18" s="1"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="6:8" ht="15.75" customHeight="1">
+    <row r="19" ht="15.75" customHeight="1">
       <c r="F19" s="4"/>
       <c r="G19" s="1"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="6:8" ht="15.75" customHeight="1">
+    <row r="20" ht="15.75" customHeight="1">
       <c r="F20" s="4"/>
       <c r="G20" s="6"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="6:8" ht="15.75" customHeight="1">
+    <row r="21" ht="15.75" customHeight="1">
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="6:8" ht="15.75" customHeight="1"/>
-    <row r="23" spans="6:8" ht="15.75" customHeight="1"/>
-    <row r="24" spans="6:8" ht="15.75" customHeight="1"/>
-    <row r="25" spans="6:8" ht="15.75" customHeight="1"/>
-    <row r="26" spans="6:8" ht="15.75" customHeight="1"/>
-    <row r="27" spans="6:8" ht="15.75" customHeight="1"/>
-    <row r="28" spans="6:8" ht="15.75" customHeight="1"/>
-    <row r="29" spans="6:8" ht="15.75" customHeight="1"/>
-    <row r="30" spans="6:8" ht="15.75" customHeight="1"/>
-    <row r="31" spans="6:8" ht="15.75" customHeight="1"/>
-    <row r="32" spans="6:8" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1"/>
+    <row r="23" ht="15.75" customHeight="1"/>
+    <row r="24" ht="15.75" customHeight="1"/>
+    <row r="25" ht="15.75" customHeight="1"/>
+    <row r="26" ht="15.75" customHeight="1"/>
+    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -4217,28 +4212,29 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="13.90625" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" customWidth="1"/>
-    <col min="3" max="6" width="12.6328125" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="13.88"/>
+    <col customWidth="1" min="2" max="2" width="16.38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4250,7 +4246,7 @@
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
     </row>
-    <row r="2" spans="1:6" ht="30.75" customHeight="1">
+    <row r="2" ht="30.75" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>37</v>
       </c>
@@ -4261,62 +4257,62 @@
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:6" ht="24.75" customHeight="1">
+    <row r="3" ht="24.75" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+    <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1"/>
+    <row r="12" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -5302,28 +5298,29 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="43.26953125" customWidth="1"/>
-    <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="6" width="12.6328125" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="43.25"/>
+    <col customWidth="1" min="2" max="2" width="40.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>39</v>
       </c>
@@ -5331,7 +5328,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1">
+    <row r="2" ht="17.25" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>37</v>
       </c>
@@ -5340,7 +5337,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>42</v>
       </c>
@@ -5351,16 +5348,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="16">
-        <v>123434</v>
+        <v>123434.0</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -5371,7 +5368,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="11" t="s">
         <v>49</v>
       </c>
@@ -5382,7 +5379,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>52</v>
       </c>
@@ -5393,18 +5390,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+    <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="9" ht="15.75" customHeight="1"/>
+    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1"/>
+    <row r="12" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -6390,28 +6387,29 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="43.26953125" customWidth="1"/>
-    <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="6" width="12.6328125" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="43.25"/>
+    <col customWidth="1" min="2" max="2" width="40.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>39</v>
       </c>
@@ -6419,7 +6417,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1">
+    <row r="2" ht="17.25" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>37</v>
       </c>
@@ -6428,7 +6426,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>42</v>
       </c>
@@ -6439,16 +6437,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="16">
-        <v>123434</v>
+        <v>123434.0</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -6459,7 +6457,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="11" t="s">
         <v>49</v>
       </c>
@@ -6470,7 +6468,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>52</v>
       </c>
@@ -6481,18 +6479,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+    <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="9" ht="15.75" customHeight="1"/>
+    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1"/>
+    <row r="12" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -7478,30 +7476,29 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="48.453125" customWidth="1"/>
-    <col min="2" max="2" width="41.08984375" customWidth="1"/>
-    <col min="3" max="6" width="12.6328125" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="48.5"/>
+    <col customWidth="1" min="2" max="2" width="41.13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
@@ -7509,7 +7506,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -7517,7 +7514,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="36" customHeight="1">
+    <row r="3" ht="36.0" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -7525,7 +7522,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="27" customHeight="1">
+    <row r="4" ht="27.0" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>57</v>
       </c>
@@ -7533,47 +7530,47 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A5" s="17" t="s">
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A6" s="17" t="s">
+    <row r="6" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A7" s="17" t="s">
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="17">
+        <v>1234567.0</v>
+      </c>
+      <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A9" s="18">
-        <v>1234567</v>
-      </c>
-      <c r="B9" s="17"/>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="17"/>
+      <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1"/>
+    <row r="12" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -8559,248 +8556,249 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="70.08984375" customWidth="1"/>
-    <col min="2" max="2" width="43.90625" customWidth="1"/>
-    <col min="3" max="3" width="41.7265625" customWidth="1"/>
-    <col min="4" max="6" width="12.6328125" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="70.13"/>
+    <col customWidth="1" min="2" max="2" width="43.88"/>
+    <col customWidth="1" min="3" max="3" width="41.75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A1" s="19" t="s">
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="20"/>
+      <c r="C1" s="19"/>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A2" s="19" t="s">
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A3" s="19" t="s">
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="19"/>
     </row>
-    <row r="4" spans="1:3" ht="49.5" customHeight="1">
-      <c r="A4" s="21" t="s">
+    <row r="4" ht="49.5" customHeight="1">
+      <c r="A4" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="21"/>
     </row>
-    <row r="5" spans="1:3" ht="52.5" customHeight="1">
-      <c r="A5" s="21" t="s">
+    <row r="5" ht="52.5" customHeight="1">
+      <c r="A5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="21"/>
     </row>
-    <row r="6" spans="1:3" ht="46.5" customHeight="1">
-      <c r="A6" s="21" t="s">
+    <row r="6" ht="46.5" customHeight="1">
+      <c r="A6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="21"/>
     </row>
-    <row r="7" spans="1:3" ht="58.5" customHeight="1">
-      <c r="A7" s="21" t="s">
+    <row r="7" ht="58.5" customHeight="1">
+      <c r="A7" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="21"/>
     </row>
-    <row r="8" spans="1:3" ht="71.25" customHeight="1">
-      <c r="A8" s="21" t="s">
+    <row r="8" ht="71.25" customHeight="1">
+      <c r="A8" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="21"/>
     </row>
-    <row r="9" spans="1:3" ht="63" customHeight="1">
-      <c r="A9" s="21" t="s">
+    <row r="9" ht="63.0" customHeight="1">
+      <c r="A9" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="21"/>
     </row>
-    <row r="10" spans="1:3" ht="156.75" customHeight="1">
-      <c r="A10" s="21" t="s">
+    <row r="10" ht="156.75" customHeight="1">
+      <c r="A10" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="21"/>
     </row>
-    <row r="11" spans="1:3" ht="156.75" customHeight="1">
-      <c r="A11" s="21" t="s">
+    <row r="11" ht="156.75" customHeight="1">
+      <c r="A11" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="22"/>
+      <c r="C11" s="21"/>
     </row>
-    <row r="12" spans="1:3" ht="162" customHeight="1">
-      <c r="A12" s="21" t="s">
+    <row r="12" ht="162.0" customHeight="1">
+      <c r="A12" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="162" customHeight="1">
-      <c r="A13" s="21" t="s">
+    <row r="13" ht="162.0" customHeight="1">
+      <c r="A13" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="162" customHeight="1">
-      <c r="A14" s="21" t="s">
+    <row r="14" ht="162.0" customHeight="1">
+      <c r="A14" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="21"/>
     </row>
-    <row r="15" spans="1:3" ht="259.5" customHeight="1">
-      <c r="A15" s="21" t="s">
+    <row r="15" ht="259.5" customHeight="1">
+      <c r="A15" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="22"/>
+      <c r="C15" s="21"/>
     </row>
-    <row r="16" spans="1:3" ht="259.5" customHeight="1">
-      <c r="A16" s="21" t="s">
+    <row r="16" ht="259.5" customHeight="1">
+      <c r="A16" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="22"/>
+      <c r="C16" s="21"/>
     </row>
-    <row r="17" spans="1:3" ht="256.5" customHeight="1">
-      <c r="A17" s="21" t="s">
+    <row r="17" ht="256.5" customHeight="1">
+      <c r="A17" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="21"/>
     </row>
-    <row r="18" spans="1:3" ht="112.5" customHeight="1">
-      <c r="A18" s="21" t="s">
+    <row r="18" ht="112.5" customHeight="1">
+      <c r="A18" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="23">
-        <v>2</v>
-      </c>
-      <c r="C18" s="22"/>
+      <c r="B18" s="22">
+        <v>2.0</v>
+      </c>
+      <c r="C18" s="21"/>
     </row>
-    <row r="19" spans="1:3" ht="112.5" customHeight="1">
-      <c r="A19" s="21" t="s">
+    <row r="19" ht="112.5" customHeight="1">
+      <c r="A19" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="22"/>
+      <c r="C19" s="21"/>
     </row>
-    <row r="20" spans="1:3" ht="103.5" customHeight="1">
-      <c r="A20" s="21" t="s">
+    <row r="20" ht="103.5" customHeight="1">
+      <c r="A20" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="22"/>
+      <c r="C20" s="21"/>
     </row>
-    <row r="21" spans="1:3" ht="138" customHeight="1">
-      <c r="A21" s="21" t="s">
+    <row r="21" ht="138.0" customHeight="1">
+      <c r="A21" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="22"/>
+      <c r="C21" s="21"/>
     </row>
-    <row r="22" spans="1:3" ht="118.5" customHeight="1">
-      <c r="A22" s="21" t="s">
+    <row r="22" ht="118.5" customHeight="1">
+      <c r="A22" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="22"/>
+      <c r="C22" s="21"/>
     </row>
-    <row r="23" spans="1:3" ht="127.5" customHeight="1">
-      <c r="A23" s="21" t="s">
+    <row r="23" ht="127.5" customHeight="1">
+      <c r="A23" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="22"/>
+      <c r="C23" s="21"/>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="24" ht="15.75" customHeight="1"/>
+    <row r="25" ht="15.75" customHeight="1"/>
+    <row r="26" ht="15.75" customHeight="1"/>
+    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -9770,7 +9768,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DsAlgo TestNG - Initial 1
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DsAlgo_TestData.xlsx
+++ b/src/test/resources/TestData/DsAlgo_TestData.xlsx
@@ -1,29 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mousu\git\DsAlgoPortal-TestNG\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41E7D74-0F5D-43C2-9136-53C0CFA5FEC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Valid_Login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Login" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Register" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Linked_List" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Graph" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Tree" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="TryEditor" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="Array" sheetId="8" r:id="rId11"/>
+    <sheet name="Valid_Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="Register" sheetId="3" r:id="rId3"/>
+    <sheet name="Linked_List" sheetId="4" r:id="rId4"/>
+    <sheet name="Graph" sheetId="5" r:id="rId5"/>
+    <sheet name="Tree" sheetId="6" r:id="rId6"/>
+    <sheet name="TryEditor" sheetId="7" r:id="rId7"/>
+    <sheet name="Array" sheetId="8" r:id="rId8"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataChecksum="2RqX7NmqtzoDWSFeiwngA9pRnP1hB2Vhhj4HR5Y8uCc="/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="110">
   <si>
     <t>username</t>
   </si>
@@ -136,18 +140,18 @@
   <si>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="10.0"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
       </rPr>
       <t>OutPut Result</t>
     </r>
@@ -254,9 +258,6 @@
     <t>my_list = [1, 2, 3]
 my_list.append(4)
 print(my_list</t>
-  </si>
-  <si>
-    <t>SyntaxError: EOF in multi-line statement on line 4</t>
   </si>
   <si>
     <t>fruits = ["apple", "banana", "cherry", "date"]
@@ -308,28 +309,6 @@
   </si>
   <si>
     <t>Some Tests failed. Please review code</t>
-  </si>
-  <si>
-    <t>def search(input_list, num): 
-if(num in input_list):
-print("Element Found")
-\b
-\b
-else:
-print("Not Found")
-\b
-\b
-\b
-\b
-search([12, 23, 45, 67, 6, 90] , 25)</t>
-  </si>
-  <si>
-    <t>Not Found</t>
-  </si>
-  <si>
-    <t>def search(lst, value):
-  return value in lst
- print(search([12, 23, 45, 67, 6, 90], 12)) #</t>
   </si>
   <si>
     <t>def search(input_list, num): 
@@ -423,17 +402,6 @@
     <t>SyntaxError: bad input on line 3</t>
   </si>
   <si>
-    <t xml:space="preserve">def sortedSquares(nums):
-\b
-\b
-\b
-\b
-return sorted(x**2 for x in nums)
-nums = [-4, -1, 0, 3, 10]
-result = sortedSquares(nums)
-print(result) </t>
-  </si>
-  <si>
     <t>[0, 1, 9, 16, 100]</t>
   </si>
   <si>
@@ -461,86 +429,143 @@
 result = sortedSquares(nums)
 print(result) # Output: [0, 1, 9, 16, 100]</t>
   </si>
+  <si>
+    <t>Arrays In Python</t>
+  </si>
+  <si>
+    <t>Arrays Using List</t>
+  </si>
+  <si>
+    <t>SyntaxError: EOF in multi-line statement on line 5</t>
+  </si>
+  <si>
+    <t>Basic Operations in Lists</t>
+  </si>
+  <si>
+    <t>Applications of Array</t>
+  </si>
+  <si>
+    <t>Search The Array</t>
+  </si>
+  <si>
+    <t>Max Consecutive Valid</t>
+  </si>
+  <si>
+    <t>Max Consecutive Submit</t>
+  </si>
+  <si>
+    <t>Max Consecutive Invalid</t>
+  </si>
+  <si>
+    <t>Find Num Valid</t>
+  </si>
+  <si>
+    <t>Find Num Submit</t>
+  </si>
+  <si>
+    <t>Find Num Invalid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def sortedSquares(nums): return sorted(x**2 for x in nums)
+nums = [-4, -1, 0, 3, 10]
+result = sortedSquares(nums)
+print(result) </t>
+  </si>
+  <si>
+    <t>Sorted Square Valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorted Square Submit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorted Square Invalid </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="15">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF467886"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF467886"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
       <b/>
-      <sz val="13.0"/>
+      <sz val="13"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="13.0"/>
+      <sz val="13"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="&quot;Aptos Narrow&quot;"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -549,11 +574,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -567,101 +598,87 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="27">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -851,21 +868,23 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -873,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -881,20 +900,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1"/>
-    <row r="4" ht="15.75" customHeight="1"/>
-    <row r="5" ht="15.75" customHeight="1"/>
-    <row r="6" ht="15.75" customHeight="1"/>
-    <row r="7" ht="15.75" customHeight="1"/>
-    <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -1880,25 +1899,23 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1906,17 +1923,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1924,7 +1941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1932,17 +1949,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1"/>
-    <row r="7" ht="15.75" customHeight="1"/>
-    <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -2928,31 +2945,29 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="18.5"/>
-    <col customWidth="1" min="3" max="3" width="19.13"/>
-    <col customWidth="1" min="4" max="4" width="34.88"/>
-    <col customWidth="1" min="5" max="5" width="50.25"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="3" max="3" width="19.08984375" customWidth="1"/>
+    <col min="4" max="4" width="34.90625" customWidth="1"/>
+    <col min="5" max="5" width="50.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2969,7 +2984,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2980,9 +2995,9 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1">
       <c r="A3" s="2">
-        <v>8.767686667E9</v>
+        <v>8767686667</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -2991,7 +3006,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3004,7 +3019,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -3016,7 +3031,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -3036,7 +3051,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -3056,7 +3071,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1">
       <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
@@ -3073,7 +3088,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>21</v>
@@ -3091,7 +3106,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -3110,15 +3125,15 @@
       <c r="F10" s="6"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="8">
-        <v>9.87654321E8</v>
+        <v>987654321</v>
       </c>
       <c r="C11" s="8">
-        <v>9.87654321E8</v>
+        <v>987654321</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>26</v>
@@ -3130,7 +3145,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -3150,7 +3165,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -3167,7 +3182,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -3185,7 +3200,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -3202,47 +3217,47 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1">
       <c r="F16" s="4"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="6:8" ht="15.75" customHeight="1">
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="6:8" ht="15.75" customHeight="1">
       <c r="F18" s="1"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="6:8" ht="15.75" customHeight="1">
       <c r="F19" s="4"/>
       <c r="G19" s="1"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="6:8" ht="15.75" customHeight="1">
       <c r="F20" s="4"/>
       <c r="G20" s="6"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="6:8" ht="15.75" customHeight="1">
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="22" spans="6:8" ht="15.75" customHeight="1"/>
+    <row r="23" spans="6:8" ht="15.75" customHeight="1"/>
+    <row r="24" spans="6:8" ht="15.75" customHeight="1"/>
+    <row r="25" spans="6:8" ht="15.75" customHeight="1"/>
+    <row r="26" spans="6:8" ht="15.75" customHeight="1"/>
+    <row r="27" spans="6:8" ht="15.75" customHeight="1"/>
+    <row r="28" spans="6:8" ht="15.75" customHeight="1"/>
+    <row r="29" spans="6:8" ht="15.75" customHeight="1"/>
+    <row r="30" spans="6:8" ht="15.75" customHeight="1"/>
+    <row r="31" spans="6:8" ht="15.75" customHeight="1"/>
+    <row r="32" spans="6:8" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -4212,29 +4227,27 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.88"/>
-    <col customWidth="1" min="2" max="2" width="16.38"/>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4246,7 +4259,7 @@
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
     </row>
-    <row r="2" ht="30.75" customHeight="1">
+    <row r="2" spans="1:6" ht="30.75" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>37</v>
       </c>
@@ -4257,62 +4270,62 @@
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" ht="24.75" customHeight="1">
+    <row r="3" spans="1:6" ht="24.75" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -5298,29 +5311,27 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="43.25"/>
-    <col customWidth="1" min="2" max="2" width="40.0"/>
+    <col min="1" max="1" width="43.26953125" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>39</v>
       </c>
@@ -5328,7 +5339,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" ht="17.25" customHeight="1">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>37</v>
       </c>
@@ -5337,7 +5348,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>42</v>
       </c>
@@ -5348,16 +5359,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="16">
-        <v>123434.0</v>
+        <v>123434</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -5368,7 +5379,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="A6" s="11" t="s">
         <v>49</v>
       </c>
@@ -5379,7 +5390,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>52</v>
       </c>
@@ -5390,18 +5401,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -6387,29 +6398,27 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="43.25"/>
-    <col customWidth="1" min="2" max="2" width="40.0"/>
+    <col min="1" max="1" width="43.26953125" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>39</v>
       </c>
@@ -6417,7 +6426,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" ht="17.25" customHeight="1">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>37</v>
       </c>
@@ -6426,7 +6435,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>42</v>
       </c>
@@ -6437,16 +6446,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="16">
-        <v>123434.0</v>
+        <v>123434</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -6457,7 +6466,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="A6" s="11" t="s">
         <v>49</v>
       </c>
@@ -6468,7 +6477,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>52</v>
       </c>
@@ -6479,18 +6488,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1"/>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -7476,29 +7485,27 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="48.5"/>
-    <col customWidth="1" min="2" max="2" width="41.13"/>
+    <col min="1" max="1" width="48.453125" customWidth="1"/>
+    <col min="2" max="2" width="41.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
@@ -7506,7 +7513,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -7514,7 +7521,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" ht="36.0" customHeight="1">
+    <row r="3" spans="1:2" ht="36" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -7522,7 +7529,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" ht="27.0" customHeight="1">
+    <row r="4" spans="1:2" ht="27" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>57</v>
       </c>
@@ -7530,7 +7537,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:2" ht="14.25" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>58</v>
       </c>
@@ -7538,7 +7545,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:2" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>60</v>
       </c>
@@ -7546,7 +7553,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>61</v>
       </c>
@@ -7554,23 +7561,23 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
       <c r="A8" s="17">
-        <v>1234567.0</v>
+        <v>1234567</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
       <c r="A9" s="17"/>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -8556,249 +8563,277 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="70.13"/>
-    <col customWidth="1" min="2" max="2" width="43.88"/>
-    <col customWidth="1" min="3" max="3" width="41.75"/>
+    <col min="1" max="1" width="70.08984375" customWidth="1"/>
+    <col min="2" max="2" width="43.90625" customWidth="1"/>
+    <col min="3" max="3" width="41.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A1" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="19"/>
+      <c r="C1" s="22"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A2" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="19"/>
+      <c r="C2" s="22" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A3" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="19"/>
+      <c r="C3" s="22" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="4" ht="49.5" customHeight="1">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:3" ht="49.5" customHeight="1">
+      <c r="A4" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="24" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="5" ht="52.5" customHeight="1">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:3" ht="52.5" customHeight="1">
+      <c r="A5" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="46.5" customHeight="1">
+      <c r="A6" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="B6" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="6" ht="46.5" customHeight="1">
-      <c r="A6" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="18" t="s">
+    <row r="7" spans="1:3" ht="58.5" customHeight="1">
+      <c r="A7" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="21"/>
+      <c r="B7" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="7" ht="58.5" customHeight="1">
-      <c r="A7" s="20" t="s">
+    <row r="8" spans="1:3" ht="71.25" customHeight="1">
+      <c r="A8" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="21"/>
+      <c r="B8" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="8" ht="71.25" customHeight="1">
-      <c r="A8" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="18" t="s">
+    <row r="9" spans="1:3" ht="63" customHeight="1">
+      <c r="A9" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="21"/>
+      <c r="B9" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="9" ht="63.0" customHeight="1">
-      <c r="A9" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="18" t="s">
+    <row r="10" spans="1:3" ht="156.75" customHeight="1">
+      <c r="A10" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="B10" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="10" ht="156.75" customHeight="1">
-      <c r="A10" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="18" t="s">
+    <row r="11" spans="1:3" ht="156.75" customHeight="1">
+      <c r="A11" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="21"/>
+      <c r="C11" s="22" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="11" ht="156.75" customHeight="1">
-      <c r="A11" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="18" t="s">
+    <row r="12" spans="1:3" ht="162" customHeight="1">
+      <c r="A12" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="B12" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="12" ht="162.0" customHeight="1">
-      <c r="A12" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="18" t="s">
+    <row r="13" spans="1:3" ht="162" customHeight="1">
+      <c r="A13" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="B13" s="25" t="s">
         <v>83</v>
       </c>
+      <c r="C13" s="22" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="13" ht="162.0" customHeight="1">
-      <c r="A13" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="21" t="s">
+    <row r="14" spans="1:3" ht="162" customHeight="1">
+      <c r="A14" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="259.5" customHeight="1">
+      <c r="A15" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="259.5" customHeight="1">
+      <c r="A16" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="26" t="s">
         <v>83</v>
       </c>
+      <c r="C16" s="22" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="14" ht="162.0" customHeight="1">
-      <c r="A14" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="21"/>
+    <row r="17" spans="1:3" ht="256.5" customHeight="1">
+      <c r="A17" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="15" ht="259.5" customHeight="1">
-      <c r="A15" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="21"/>
+    <row r="18" spans="1:3" ht="112.5" customHeight="1">
+      <c r="A18" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="16" ht="259.5" customHeight="1">
-      <c r="A16" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="21"/>
+    <row r="19" spans="1:3" ht="112.5" customHeight="1">
+      <c r="A19" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>107</v>
+      </c>
     </row>
-    <row r="17" ht="256.5" customHeight="1">
-      <c r="A17" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" s="21"/>
+    <row r="20" spans="1:3" ht="103.5" customHeight="1">
+      <c r="A20" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="18" ht="112.5" customHeight="1">
-      <c r="A18" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" s="22">
-        <v>2.0</v>
-      </c>
-      <c r="C18" s="21"/>
+    <row r="21" spans="1:3" ht="138" customHeight="1">
+      <c r="A21" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="19" ht="112.5" customHeight="1">
-      <c r="A19" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="21"/>
+    <row r="22" spans="1:3" ht="118.5" customHeight="1">
+      <c r="A22" s="19"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="20"/>
     </row>
-    <row r="20" ht="103.5" customHeight="1">
-      <c r="A20" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20" s="21"/>
+    <row r="23" spans="1:3" ht="127.5" customHeight="1">
+      <c r="A23" s="19"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="20"/>
     </row>
-    <row r="21" ht="138.0" customHeight="1">
-      <c r="A21" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="21"/>
-    </row>
-    <row r="22" ht="118.5" customHeight="1">
-      <c r="A22" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="21"/>
-    </row>
-    <row r="23" ht="127.5" customHeight="1">
-      <c r="A23" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="21"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -9768,9 +9803,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>